<commit_message>
Added graph. But need to be formatted
</commit_message>
<xml_diff>
--- a/inst/extdata/enrollments.xlsx
+++ b/inst/extdata/enrollments.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Windows\Analytics\R Programming\GitHub\App\clinicalDashboard\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Windows\Analytics\R Programming\GitHub\App\golem\clinicalDashboard\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF2F2D0-1706-4CB9-8284-DADB249FA8C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9B58A9-4A4E-488D-A18F-3D31991E4F58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" xr2:uid="{2AE06771-101C-4AE5-AA7C-FF60A3769190}"/>
   </bookViews>
@@ -1907,7 +1907,7 @@
         <v>26</v>
       </c>
       <c r="C50" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D50" t="s">
         <v>12</v>
@@ -3009,7 +3009,7 @@
         <v>25</v>
       </c>
       <c r="C88" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D88" t="s">
         <v>12</v>
@@ -3502,7 +3502,7 @@
         <v>21</v>
       </c>
       <c r="C105" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D105" t="s">
         <v>12</v>
@@ -6257,7 +6257,7 @@
         <v>10</v>
       </c>
       <c r="C200" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D200" t="s">
         <v>12</v>
@@ -6460,7 +6460,7 @@
         <v>10</v>
       </c>
       <c r="C207" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D207" t="s">
         <v>12</v>
@@ -8954,7 +8954,7 @@
         <v>25</v>
       </c>
       <c r="C293" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D293" t="s">
         <v>12</v>
@@ -8983,7 +8983,7 @@
         <v>10</v>
       </c>
       <c r="C294" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D294" t="s">
         <v>12</v>
@@ -11535,7 +11535,7 @@
         <v>21</v>
       </c>
       <c r="C382" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D382" t="s">
         <v>12</v>
@@ -11999,7 +11999,7 @@
         <v>10</v>
       </c>
       <c r="C398" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D398" t="s">
         <v>12</v>
@@ -12086,7 +12086,7 @@
         <v>25</v>
       </c>
       <c r="C401" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D401" t="s">
         <v>16</v>
@@ -13014,7 +13014,7 @@
         <v>21</v>
       </c>
       <c r="C433" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D433" t="s">
         <v>12</v>
@@ -13188,7 +13188,7 @@
         <v>26</v>
       </c>
       <c r="C439" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D439" t="s">
         <v>16</v>
@@ -13884,7 +13884,7 @@
         <v>21</v>
       </c>
       <c r="C463" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D463" t="s">
         <v>12</v>
@@ -14522,7 +14522,7 @@
         <v>21</v>
       </c>
       <c r="C485" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D485" t="s">
         <v>12</v>
@@ -14841,7 +14841,7 @@
         <v>25</v>
       </c>
       <c r="C496" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D496" t="s">
         <v>12</v>
@@ -14979,7 +14979,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I1" xr:uid="{3358A548-6214-42EB-BF92-7267BFFCA0A9}"/>
+  <autoFilter ref="A1:I1" xr:uid="{39096195-16AB-4643-9D6A-A5D916737B45}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>